<commit_message>
add reviewed_at and escalated_to columns to close #25
</commit_message>
<xml_diff>
--- a/inst/example_data/measure_config.xlsx
+++ b/inst/example_data/measure_config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.smith5\OneDrive - nuh.nhs.uk\Documents\R\R Package Development\ThomUK\SPCreporter\inst\example_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Tom Smith\Documents\R\R Projects\SPCreporter\dev_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DD2368D-C1A5-4DB9-A9CE-1855B227BA0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16305" windowHeight="3585"/>
+    <workbookView xWindow="756" yWindow="768" windowWidth="21624" windowHeight="11244" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="measure_config" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="49">
   <si>
     <t>ARGR</t>
   </si>
@@ -150,12 +151,33 @@
   </si>
   <si>
     <t>Answers per day</t>
+  </si>
+  <si>
+    <t>reviewed_at</t>
+  </si>
+  <si>
+    <t>escalated_to</t>
+  </si>
+  <si>
+    <t>Division Performance</t>
+  </si>
+  <si>
+    <t>Trust Performance</t>
+  </si>
+  <si>
+    <t>HR Review</t>
+  </si>
+  <si>
+    <t>Board</t>
+  </si>
+  <si>
+    <t>Directorate Performance</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -466,29 +488,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" customWidth="1"/>
+    <col min="6" max="6" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -505,31 +529,37 @@
         <v>35</v>
       </c>
       <c r="F1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" t="s">
         <v>33</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" t="s">
         <v>32</v>
       </c>
-      <c r="I1" t="s">
+      <c r="K1" t="s">
         <v>31</v>
       </c>
-      <c r="J1" t="s">
+      <c r="L1" t="s">
         <v>30</v>
       </c>
-      <c r="K1" t="s">
+      <c r="M1" t="s">
         <v>29</v>
       </c>
-      <c r="L1" t="s">
+      <c r="N1" t="s">
         <v>28</v>
       </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -543,19 +573,25 @@
         <v>5</v>
       </c>
       <c r="F2" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" t="s">
+        <v>45</v>
+      </c>
+      <c r="H2" t="s">
         <v>25</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>23</v>
       </c>
-      <c r="K2">
+      <c r="M2">
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
@@ -572,25 +608,31 @@
         <v>4</v>
       </c>
       <c r="F3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H3" t="s">
         <v>10</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>22</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <v>0.69691733109252596</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>21</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>20</v>
       </c>
-      <c r="K3">
+      <c r="M3">
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
@@ -607,25 +649,31 @@
         <v>4</v>
       </c>
       <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H4" t="s">
         <v>3</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
         <v>2</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>0.70831026663978502</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>1</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>19</v>
       </c>
-      <c r="K4">
+      <c r="M4">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>11</v>
       </c>
@@ -642,22 +690,28 @@
         <v>16</v>
       </c>
       <c r="F5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+      <c r="H5" t="s">
         <v>3</v>
       </c>
-      <c r="G5" t="s">
+      <c r="I5" t="s">
         <v>2</v>
       </c>
-      <c r="I5" t="s">
+      <c r="K5" t="s">
         <v>1</v>
       </c>
-      <c r="J5" t="s">
+      <c r="L5" t="s">
         <v>15</v>
       </c>
-      <c r="K5">
+      <c r="M5">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>16</v>
       </c>
@@ -674,25 +728,31 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" t="s">
+      <c r="I6" t="s">
         <v>2</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>0.9</v>
       </c>
-      <c r="I6" t="s">
+      <c r="K6" t="s">
         <v>9</v>
       </c>
-      <c r="J6" t="s">
+      <c r="L6" t="s">
         <v>8</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>43</v>
       </c>
@@ -709,21 +769,27 @@
         <v>4</v>
       </c>
       <c r="F7" t="s">
+        <v>48</v>
+      </c>
+      <c r="G7" t="s">
+        <v>44</v>
+      </c>
+      <c r="H7" t="s">
         <v>3</v>
       </c>
-      <c r="G7" t="s">
+      <c r="I7" t="s">
         <v>2</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>0.48580767330449598</v>
       </c>
-      <c r="I7" t="s">
+      <c r="K7" t="s">
         <v>1</v>
       </c>
-      <c r="J7" t="s">
+      <c r="L7" t="s">
         <v>0</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add reviewed_at and escalated_to columns
</commit_message>
<xml_diff>
--- a/inst/example_data/measure_config.xlsx
+++ b/inst/example_data/measure_config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thomas.smith5\OneDrive - nuh.nhs.uk\Documents\R\R Package Development\ThomUK\SPCreporter\inst\example_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\Tom Smith\Documents\R\R Projects\SPCreporter\inst\example_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7513E22-A882-461A-BA55-64CC7049B007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16305" windowHeight="3585"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="measure_config" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
   <si>
     <t>ARGR</t>
   </si>
@@ -150,12 +151,27 @@
   </si>
   <si>
     <t>Answers per day</t>
+  </si>
+  <si>
+    <t>allowable_days_lag</t>
+  </si>
+  <si>
+    <t>reviewed_at</t>
+  </si>
+  <si>
+    <t>escalated_to</t>
+  </si>
+  <si>
+    <t>Divisional perfomance meeting</t>
+  </si>
+  <si>
+    <t>Service performance meeting</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -466,29 +482,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.28515625" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="4" max="4" width="26.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" customWidth="1"/>
+    <col min="7" max="7" width="22.5546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="26.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -528,8 +545,17 @@
       <c r="M1" t="s">
         <v>27</v>
       </c>
+      <c r="N1" t="s">
+        <v>42</v>
+      </c>
+      <c r="O1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -555,7 +581,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>5</v>
       </c>
@@ -589,8 +615,14 @@
       <c r="K3">
         <v>24</v>
       </c>
+      <c r="O3" t="s">
+        <v>46</v>
+      </c>
+      <c r="P3" t="s">
+        <v>45</v>
+      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10</v>
       </c>
@@ -625,7 +657,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>11</v>
       </c>
@@ -657,7 +689,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>16</v>
       </c>
@@ -692,7 +724,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>43</v>
       </c>

</xml_diff>

<commit_message>
Update internal example data to include rare_events flag
</commit_message>
<xml_diff>
--- a/inst/example_data/measure_config.xlsx
+++ b/inst/example_data/measure_config.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2250" windowWidth="16305" windowHeight="3585"/>
+    <workbookView xWindow="0" yWindow="2700" windowWidth="16305" windowHeight="3585"/>
   </bookViews>
   <sheets>
     <sheet name="measure_config" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="50">
   <si>
     <t>ARGR</t>
   </si>
@@ -155,16 +155,25 @@
     <t>Problems</t>
   </si>
   <si>
-    <t>"2020-04-01"</t>
-  </si>
-  <si>
-    <t>rare_event_chart</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Y</t>
+    <t>allowable_days_lag</t>
+  </si>
+  <si>
+    <t>reviewed_at</t>
+  </si>
+  <si>
+    <t>escalated_to</t>
+  </si>
+  <si>
+    <t>"2020-04-27"</t>
+  </si>
+  <si>
+    <t>Rebased to demonstrate the method.  Add the rebase_dates and rebase_comment to 'measure_config.xlsx'.</t>
+  </si>
+  <si>
+    <t>Service performance meeting</t>
+  </si>
+  <si>
+    <t>Divisional perfomance meeting</t>
   </si>
 </sst>
 </file>
@@ -482,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N8"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,16 +503,19 @@
     <col min="3" max="3" width="15.85546875" customWidth="1"/>
     <col min="4" max="4" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="30.28515625" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21.5703125" customWidth="1"/>
+    <col min="15" max="15" width="26.85546875" customWidth="1"/>
+    <col min="16" max="16" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>39</v>
       </c>
@@ -523,31 +535,37 @@
         <v>34</v>
       </c>
       <c r="G1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M1" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" t="s">
+        <v>43</v>
+      </c>
+      <c r="O1" t="s">
         <v>44</v>
       </c>
-      <c r="H1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I1" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" t="s">
-        <v>31</v>
-      </c>
-      <c r="K1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N1" t="s">
-        <v>27</v>
+      <c r="P1" t="s">
+        <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -564,19 +582,22 @@
         <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>45</v>
-      </c>
-      <c r="H2" t="s">
         <v>24</v>
       </c>
-      <c r="K2" t="s">
+      <c r="J2" t="s">
         <v>23</v>
       </c>
-      <c r="L2">
+      <c r="K2">
         <v>24</v>
       </c>
+      <c r="L2" t="s">
+        <v>46</v>
+      </c>
+      <c r="M2" t="s">
+        <v>47</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>5</v>
       </c>
@@ -596,28 +617,28 @@
         <v>10</v>
       </c>
       <c r="G3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H3" t="s">
         <v>22</v>
       </c>
-      <c r="I3">
+      <c r="H3">
         <v>0.69691733109252596</v>
       </c>
+      <c r="I3" t="s">
+        <v>21</v>
+      </c>
       <c r="J3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" t="s">
         <v>20</v>
       </c>
-      <c r="L3">
+      <c r="K3">
         <v>24</v>
       </c>
-      <c r="M3" t="s">
-        <v>43</v>
+      <c r="O3" t="s">
+        <v>48</v>
+      </c>
+      <c r="P3" t="s">
+        <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
@@ -637,25 +658,22 @@
         <v>3</v>
       </c>
       <c r="G4" t="s">
-        <v>45</v>
-      </c>
-      <c r="H4" t="s">
         <v>2</v>
       </c>
-      <c r="I4">
+      <c r="H4">
         <v>0.70831026663978502</v>
       </c>
+      <c r="I4" t="s">
+        <v>1</v>
+      </c>
       <c r="J4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4" t="s">
         <v>19</v>
       </c>
-      <c r="L4">
+      <c r="K4">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>11</v>
       </c>
@@ -675,22 +693,19 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>45</v>
-      </c>
-      <c r="H5" t="s">
         <v>2</v>
       </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
       <c r="J5" t="s">
-        <v>1</v>
-      </c>
-      <c r="K5" t="s">
         <v>15</v>
       </c>
-      <c r="L5">
+      <c r="K5">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>16</v>
       </c>
@@ -710,25 +725,22 @@
         <v>10</v>
       </c>
       <c r="G6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" t="s">
         <v>2</v>
       </c>
-      <c r="I6">
+      <c r="H6">
         <v>0.9</v>
       </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
       <c r="J6" t="s">
-        <v>9</v>
-      </c>
-      <c r="K6" t="s">
         <v>8</v>
       </c>
-      <c r="L6">
+      <c r="K6">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>43</v>
       </c>
@@ -748,25 +760,22 @@
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>45</v>
-      </c>
-      <c r="H7" t="s">
         <v>2</v>
       </c>
-      <c r="I7">
+      <c r="H7">
         <v>0.48580767330449598</v>
       </c>
+      <c r="I7" t="s">
+        <v>1</v>
+      </c>
       <c r="J7" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" t="s">
         <v>0</v>
       </c>
-      <c r="L7">
+      <c r="K7">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>99</v>
       </c>
@@ -783,21 +792,18 @@
         <v>25</v>
       </c>
       <c r="G8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" t="s">
         <v>22</v>
       </c>
-      <c r="I8">
+      <c r="H8">
         <v>0</v>
       </c>
+      <c r="I8" t="s">
+        <v>1</v>
+      </c>
       <c r="J8" t="s">
-        <v>1</v>
-      </c>
-      <c r="K8" t="s">
         <v>8</v>
       </c>
-      <c r="L8">
+      <c r="K8">
         <v>24</v>
       </c>
     </row>

</xml_diff>